<commit_message>
corregiu caminho das planilhas, add as baixa de empresa no contole
</commit_message>
<xml_diff>
--- a/braspress/planilha_braspres.xlsx
+++ b/braspress/planilha_braspres.xlsx
@@ -664,7 +664,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Período: 30/09/2025 até 20/10/2025</t>
+          <t>Período: 03/10/2025 até 23/10/2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -1550,7 +1550,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Data: 20/10/2025 21:45</t>
+          <t>Data: 23/10/2025 22:03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>

</xml_diff>

<commit_message>
add email do dos representantes de vendas
</commit_message>
<xml_diff>
--- a/braspress/planilha_braspres.xlsx
+++ b/braspress/planilha_braspres.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,7 +664,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Período: 05/10/2025 até 25/10/2025</t>
+          <t>Período: 20/10/2025 até 09/11/2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -863,12 +863,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">151709, </t>
+          <t xml:space="preserve">8809, </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3724946</t>
+          <t>3755908</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -878,27 +878,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10285063000195</t>
+          <t>10285063000276</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>MJ COMERCIO E SERVICOS DE INFORMATICA E</t>
+          <t>MJ COMERCIO E SERVICOS DE INFORMATICA E TELECOMUNICACOES LTD</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>6043130000198</t>
+          <t>2952192000161</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>COLECAO INDUSTRIA E COMERCIO DE INFORMATICA, TELECOMUNICACOE</t>
+          <t>CABO SERVICOS DE TELECOMUNICACOES LTDA</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>13/10/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -908,12 +908,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>21/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>21/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>20/10/2025</t>
+          <t>08/11/2025</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>FORTALEZA</t>
+          <t>EUSEBIO</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -953,22 +953,22 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>VAG</t>
+          <t>NAT</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>VARGINHA</t>
+          <t>NATAL</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>RN</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>104,91</t>
+          <t>117,50</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>4,34</t>
+          <t>33,00</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -988,24 +988,24 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>350,00</t>
+          <t>5.829,00</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>https://www.braspress.com.br/w/tracking/search?cnpj=10285063000195&amp;documentType=CONHECIMENTO&amp;numero=3724946</t>
+          <t>https://www.braspress.com.br/w/tracking/search?cnpj=10285063000276&amp;documentType=CONHECIMENTO&amp;numero=3755908</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">151515, </t>
+          <t xml:space="preserve">153161, </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3721810</t>
+          <t>3755909</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1025,17 +1025,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2519126000100</t>
+          <t>10483444002556</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>CYBERMAX COMPUTADORES LTDA</t>
+          <t>BETANIA LACTEOS S.A.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>09/10/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1045,27 +1045,27 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>20/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>20/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>FINALIZADO</t>
+          <t>AWB EM VIAGEM</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>ENTREGA REALIZADA</t>
+          <t>LIBERACAO DE OCORR. NA EMISSAO</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>14/10/2025</t>
+          <t>06/11/2025</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1090,22 +1090,22 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>CCT</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>SAO PAULO</t>
+          <t>SALVADOR</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>91,33</t>
+          <t>260,51</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>11,02</t>
+          <t>48,72</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1125,50 +1125,158 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>563,00</t>
+          <t>12.576,00</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>https://www.braspress.com.br/w/tracking/search?cnpj=10285063000195&amp;documentType=CONHECIMENTO&amp;numero=3721810</t>
+          <t>https://www.braspress.com.br/w/tracking/search?cnpj=10285063000195&amp;documentType=CONHECIMENTO&amp;numero=3755909</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total de Conhecimentos: 2</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
+          <t xml:space="preserve">152553, </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>3740043</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>10285063000195</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MJ COMERCIO E SERVICOS DE INFORMATICA E</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2519126000100</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>CYBERMAX COMPUTADORES LTDA</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>27/10/2025</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>DANFE</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>05/11/2025</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>05/11/2025</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>FINALIZADO</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>ENTREGA REALIZADA</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>04/11/2025</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>RODO</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>FOR</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>FORTALEZA</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>CCT</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>SAO PAULO</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>90,01</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>12,00</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>11,00</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>532,52</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>https://www.braspress.com.br/w/tracking/search?cnpj=10285063000195&amp;documentType=CONHECIMENTO&amp;numero=3740043</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total de Conhecimentos: 3</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1226,11 +1334,7 @@
       <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Parâmetros:</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -1261,7 +1365,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Status: Todos</t>
+          <t>Parâmetros:</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1294,7 +1398,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pesquisar como Grupo de Empresa: Sim</t>
+          <t>Status: Todos</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1327,7 +1431,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UF Destino: Todos</t>
+          <t>Pesquisar como Grupo de Empresa: Sim</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1360,7 +1464,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Modal: Rodoviário</t>
+          <t>UF Destino: Todos</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1393,7 +1497,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Pesquiar Por: Remetente</t>
+          <t>Modal: Rodoviário</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1424,7 +1528,11 @@
       <c r="AA18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Pesquiar Por: Remetente</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
@@ -1482,11 +1590,7 @@
       <c r="AA20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Observação:</t>
-        </is>
-      </c>
+      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
@@ -1517,7 +1621,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Utiliza dados, referente às emissões efetivadas até o momento da extração deste relatório.</t>
+          <t>Observação:</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1550,7 +1654,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Data: 25/10/2025 09:57</t>
+          <t>Utiliza dados, referente às emissões efetivadas até o momento da extração deste relatório.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1580,6 +1684,39 @@
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Data: 09/11/2025 12:49</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add nome campo de cliente no json
</commit_message>
<xml_diff>
--- a/braspress/planilha_braspres.xlsx
+++ b/braspress/planilha_braspres.xlsx
@@ -664,7 +664,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Período: 21/10/2025 até 10/11/2025</t>
+          <t>Período: 22/10/2025 até 11/11/2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CABO SERVICOS DE TELECOMUNICACOES LTDA</t>
+          <t>ALARES INTERNET S A</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>MJ COMERCIO E SERVICOS DE INFORMATICA E</t>
+          <t>MJ COMERCIO E SERV DE INF E TELECOMUNICA</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1055,17 +1055,17 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>AWB EM VIAGEM</t>
+          <t>FINALIZADO</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>MALOTE LIBERADO POSTO FISCAL</t>
+          <t>ENTREGA REALIZADA</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>MJ COMERCIO E SERVICOS DE INFORMATICA E</t>
+          <t>MJ COMERCIO E SERV DE INF E TELECOMUNICA</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1687,7 +1687,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Data: 10/11/2025 22:37</t>
+          <t>Data: 11/11/2025 22:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>

</xml_diff>